<commit_message>
fix: update filename for carga antecipadas in saving_calculator.py
</commit_message>
<xml_diff>
--- a/data/Cargas_Antecipadas.xlsx
+++ b/data/Cargas_Antecipadas.xlsx
@@ -132,7 +132,7 @@
   <numFmts count="3">
     <numFmt numFmtId="44" formatCode="_-&quot;R$&quot;\ * #,##0.00_-;\-&quot;R$&quot;\ * #,##0.00_-;_-&quot;R$&quot;\ * &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="164" formatCode="d/m/yy\ h:mm;@"/>
-    <numFmt numFmtId="169" formatCode="dd/mm/yy;@"/>
+    <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
   </numFmts>
   <fonts count="6" x14ac:knownFonts="1">
     <font>
@@ -226,7 +226,7 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="169" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -415,7 +415,7 @@
         <family val="2"/>
         <scheme val="minor"/>
       </font>
-      <numFmt numFmtId="169" formatCode="dd/mm/yy;@"/>
+      <numFmt numFmtId="165" formatCode="dd/mm/yy;@"/>
       <fill>
         <patternFill patternType="none">
           <fgColor indexed="64"/>
@@ -523,6 +523,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -863,7 +867,7 @@
   <dimension ref="A1:J473"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2614,6 +2618,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <data xmlns="f9b758c5-f800-40a0-9131-e6df86a3782b" xsi:nil="true"/>
+    <TaxCatchAll xmlns="23679928-854d-4521-a60e-9e6c78a16dd1" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f9b758c5-f800-40a0-9131-e6df86a3782b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100BB5A334695902545BD40CABEF8C52A3D" ma:contentTypeVersion="14" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="eb06f967eb6492a8753cd534c679e74f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="f9b758c5-f800-40a0-9131-e6df86a3782b" xmlns:ns3="23679928-854d-4521-a60e-9e6c78a16dd1" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="30a4a470df8b7c8fe69689e3d882ba89" ns2:_="" ns3:_="">
     <xsd:import namespace="f9b758c5-f800-40a0-9131-e6df86a3782b"/>
@@ -2842,28 +2867,26 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E4090C1-1A55-4D93-9CBD-84D568E1C335}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f9b758c5-f800-40a0-9131-e6df86a3782b"/>
+    <ds:schemaRef ds:uri="23679928-854d-4521-a60e-9e6c78a16dd1"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <data xmlns="f9b758c5-f800-40a0-9131-e6df86a3782b" xsi:nil="true"/>
-    <TaxCatchAll xmlns="23679928-854d-4521-a60e-9e6c78a16dd1" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f9b758c5-f800-40a0-9131-e6df86a3782b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{300A78D9-2034-4DC3-87ED-A5EDD0279F2F}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1157B0F4-A5CB-4975-A4A2-A3B134590E30}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2880,23 +2903,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{300A78D9-2034-4DC3-87ED-A5EDD0279F2F}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8E4090C1-1A55-4D93-9CBD-84D568E1C335}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f9b758c5-f800-40a0-9131-e6df86a3782b"/>
-    <ds:schemaRef ds:uri="23679928-854d-4521-a60e-9e6c78a16dd1"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>